<commit_message>
get timezones on country in lead form
</commit_message>
<xml_diff>
--- a/excel_data/Book38.xlsx
+++ b/excel_data/Book38.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97016F98-0C1F-4DD7-8EE8-33BB14B46699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TME-1\excel_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0011ADEC-5A52-4BF1-9449-23125664C601}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD099A39-A086-4377-802D-B27D655D95FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BD099A39-A086-4377-802D-B27D655D95FF}"/>
   </bookViews>
   <sheets>
     <sheet name="masterlead" sheetId="1" r:id="rId1"/>
@@ -18,17 +23,162 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tejaswi Dessai</author>
+  </authors>
+  <commentList>
+    <comment ref="P104" authorId="0" shapeId="0" xr:uid="{0E15AEBE-DA62-431A-9F22-0A662BCF94F4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tejaswi Dessai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Removed Default Null</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P105" authorId="0" shapeId="0" xr:uid="{3140CE06-C833-44E7-98E5-5AC08EC69B6A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tejaswi Dessai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Removed Default Null</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P106" authorId="0" shapeId="0" xr:uid="{F9736A35-DE71-4DE1-B15B-E6E66110AA89}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tejaswi Dessai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Removed Default Null</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P107" authorId="0" shapeId="0" xr:uid="{EEC47561-5D83-4112-AF92-B4820D4912F2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tejaswi Dessai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Removed Default Null</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P108" authorId="0" shapeId="0" xr:uid="{7BA9EBC1-97AC-4EE1-BC31-785C2B23320B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tejaswi Dessai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Removed Default Null</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P109" authorId="0" shapeId="0" xr:uid="{F4AD4651-0B2C-49F6-A43D-47EC697AE167}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tejaswi Dessai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Removed Default Null</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1177,9 +1327,6 @@
     <t>cvdisp</t>
   </si>
   <si>
-    <t>null = default, 1=live, 0=dead</t>
-  </si>
-  <si>
     <t>Agent ID_I</t>
   </si>
   <si>
@@ -1584,12 +1731,15 @@
   <si>
     <t>constraint composnmlk unique(fname, lname, plink)</t>
   </si>
+  <si>
+    <t>1=yes, 0=Default</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1623,8 +1773,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1667,6 +1830,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1689,7 +1858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1708,6 +1877,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2992,36 +3162,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BB87AE-BC89-4D1B-A655-CF0191129AC5}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:T166"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BB87AE-BC89-4D1B-A655-CF0191129AC5}">
+  <dimension ref="A1:T162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="70" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="E88" zoomScale="70" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P104" sqref="P104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.08984375" customWidth="1"/>
-    <col min="16" max="16" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="75.81640625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="75.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3074,7 +3243,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3109,7 +3278,7 @@
         <v>lmid integer GENERATED ALWAYS AS IDENTITY (INCREMENT 1) primary key,</v>
       </c>
     </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3145,7 +3314,7 @@
         <v>rlc smallint check (rlc &gt;=0 and rlc &lt;=1),</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -3186,7 +3355,7 @@
         <v>ontag smallint check (ontag &gt;=0 and ontag &lt;=1),</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -3234,7 +3403,7 @@
         <v>cnid integer,</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -3264,7 +3433,7 @@
         <v>campgrp varchar (100),</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -3312,7 +3481,7 @@
         <v>agent integer,</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -3360,7 +3529,7 @@
         <v>sal varchar (10) not null,</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -3409,7 +3578,7 @@
         <v>fname varchar (100) not null,</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -3458,7 +3627,7 @@
         <v>lname varchar (100) not null,</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -3489,7 +3658,7 @@
         <v>conname varchar (100),</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -3537,7 +3706,7 @@
         <v>jtitle varchar (150) not null,</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -3591,7 +3760,7 @@
         <v xml:space="preserve">Jlevel smallint not null, </v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -3642,7 +3811,7 @@
         <v xml:space="preserve">dname smallint not null, </v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -3687,7 +3856,7 @@
         <v>cname varchar (150) not null,</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -3731,7 +3900,7 @@
         <v>ctyp smallint check (ctyp &gt;=0 and ctyp &lt;=4),</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -3782,7 +3951,7 @@
         <v>email varchar (150) unique not null,</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -3827,7 +3996,7 @@
         <v>phone integer not null,</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -3874,7 +4043,7 @@
         <v>linetype smallint check (linetype &gt;=0 and linetype &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -3916,7 +4085,7 @@
         <v>phext integer,</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -3961,7 +4130,7 @@
         <v>altphn varchar (50),</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -4003,7 +4172,7 @@
         <v>address varchar (255) not null,</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -4045,7 +4214,7 @@
         <v>city varchar (100) not null,</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -4087,7 +4256,7 @@
         <v>state varchar (100) not null,</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -4129,7 +4298,7 @@
         <v>zipcode varchar (20) not null,</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -4174,7 +4343,7 @@
         <v xml:space="preserve">country smallint not null, </v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -4219,7 +4388,7 @@
         <v xml:space="preserve">timez smallint not null, </v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -4267,7 +4436,7 @@
         <v>indtry integer not null,</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -4315,7 +4484,7 @@
         <v>sindtry integer not null,</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -4359,7 +4528,7 @@
         <v>sectyp smallint check (sectyp &gt;=0 and sectyp &lt;=4),</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4401,7 +4570,7 @@
         <v>empsize integer,</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -4437,7 +4606,7 @@
         <v>arevenue integer,</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -4478,7 +4647,7 @@
         <v>mlbl smallint check (mlbl &gt;=0 and mlbl &lt;=4),</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -4523,7 +4692,7 @@
         <v>curr integer,</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -4565,7 +4734,7 @@
         <v>domain varchar (255) not null,</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>103</v>
       </c>
@@ -4614,7 +4783,7 @@
         <v>plink varchar (800) unique not null,</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -4656,7 +4825,7 @@
         <v>empszlink varchar (800) not null,</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -4701,7 +4870,7 @@
         <v>indlink varchar (800) not null,</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -4746,7 +4915,7 @@
         <v>revszlink varchar (800) not null,</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -4785,8 +4954,7 @@
         <v>othrlink varchar (800),</v>
       </c>
     </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -4822,7 +4990,7 @@
         <v>svagtidi integer,</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -4849,7 +5017,7 @@
         <v>svdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -4888,7 +5056,7 @@
         <v>stagtidi integer,</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -4918,7 +5086,7 @@
         <v>stdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -4957,7 +5125,7 @@
         <v>stagtidii integer,</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -4987,7 +5155,7 @@
         <v>stdtii timestamp without time zone,</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -5020,7 +5188,7 @@
         <v>sbsvtag integer,</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -5056,7 +5224,7 @@
         <v>pcomt varchar (255),</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -5091,7 +5259,7 @@
         <v>pctag smallint check (pctag &gt;=0 and pctag &lt;=2),</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -5126,7 +5294,7 @@
         <v>pcmandt smallint check (pcmandt &gt;=0 and pcmandt &lt;=1),</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -5158,9 +5326,9 @@
         <v>pload smallint check (pload &gt;=0 and pload &lt;=1),</v>
       </c>
     </row>
-    <row r="53" spans="1:20" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>221</v>
       </c>
@@ -5196,7 +5364,7 @@
         <v>dvagtidi integer,</v>
       </c>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>221</v>
       </c>
@@ -5223,7 +5391,7 @@
         <v>dvdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>221</v>
       </c>
@@ -5259,7 +5427,7 @@
         <v>dvagtidii integer,</v>
       </c>
     </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>221</v>
       </c>
@@ -5286,7 +5454,7 @@
         <v>dvdtii timestamp without time zone,</v>
       </c>
     </row>
-    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>221</v>
       </c>
@@ -5313,7 +5481,7 @@
         <v>dvrdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>221</v>
       </c>
@@ -5349,7 +5517,7 @@
         <v>dvragtidi integer,</v>
       </c>
     </row>
-    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>221</v>
       </c>
@@ -5376,7 +5544,7 @@
         <v>dvrdtii timestamp without time zone,</v>
       </c>
     </row>
-    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>221</v>
       </c>
@@ -5412,7 +5580,7 @@
         <v>dvragtidii integer,</v>
       </c>
     </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>221</v>
       </c>
@@ -5443,7 +5611,7 @@
         <v>dvrejtg smallint check (dvrejtg &gt;=0 and dvrejtg &lt;=3),</v>
       </c>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>221</v>
       </c>
@@ -5474,7 +5642,7 @@
         <v>dvsbtg smallint check (dvsbtg &gt;=0 and dvsbtg &lt;=3),</v>
       </c>
     </row>
-    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>221</v>
       </c>
@@ -5504,7 +5672,7 @@
         <v>dvrejectreason varchar (100),</v>
       </c>
     </row>
-    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>221</v>
       </c>
@@ -5537,7 +5705,7 @@
         <v>dvcomt varchar (255),</v>
       </c>
     </row>
-    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>221</v>
       </c>
@@ -5572,7 +5740,7 @@
         <v>dvstat smallint check (dvstat &gt;=0 and dvstat &lt;=2),</v>
       </c>
     </row>
-    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>221</v>
       </c>
@@ -5604,9 +5772,9 @@
         <v>dvload smallint check (dvload &gt;=0 and dvload &lt;=1),</v>
       </c>
     </row>
-    <row r="69" spans="1:20" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="71" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>255</v>
       </c>
@@ -5655,7 +5823,7 @@
         <v>evdisp smallint check (evdisp &gt;=0 and evdisp &lt;=6) not null,</v>
       </c>
     </row>
-    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>255</v>
       </c>
@@ -5696,7 +5864,7 @@
         <v>evstat smallint check (evstat &gt;=0 and evstat &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>255</v>
       </c>
@@ -5741,7 +5909,7 @@
         <v>evmail varchar (150) not null,</v>
       </c>
     </row>
-    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>255</v>
       </c>
@@ -5780,7 +5948,7 @@
         <v>evagti integer,</v>
       </c>
     </row>
-    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>255</v>
       </c>
@@ -5810,7 +5978,7 @@
         <v>evdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>255</v>
       </c>
@@ -5849,7 +6017,7 @@
         <v>evagtii integer,</v>
       </c>
     </row>
-    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>255</v>
       </c>
@@ -5879,7 +6047,7 @@
         <v>evdtii timestamp without time zone,</v>
       </c>
     </row>
-    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>255</v>
       </c>
@@ -5914,7 +6082,7 @@
         <v>evcomp smallint check (evcomp &gt;=0 and evcomp &lt;=2),</v>
       </c>
     </row>
-    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>255</v>
       </c>
@@ -5949,9 +6117,9 @@
         <v>evload smallint check (evload &gt;=0 and evload &lt;=1),</v>
       </c>
     </row>
-    <row r="80" spans="1:20" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>287</v>
       </c>
@@ -5990,7 +6158,7 @@
         <v>lcalldisp varchar (25),</v>
       </c>
     </row>
-    <row r="83" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>287</v>
       </c>
@@ -6028,7 +6196,7 @@
         <v>lcallstat smallint check (lcallstat &gt;=0 and lcallstat &lt;=2),</v>
       </c>
     </row>
-    <row r="84" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>287</v>
       </c>
@@ -6069,7 +6237,7 @@
         <v>ddispositionclass smallint check (ddispositionclass &gt;=0 and ddispositionclass &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="85" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>287</v>
       </c>
@@ -6110,7 +6278,7 @@
         <v>cvr smallint check (cvr &gt;=0 and cvr &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>303</v>
       </c>
@@ -6154,7 +6322,7 @@
         <v>emailver smallint check (emailver &gt;=0 and emailver &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>287</v>
       </c>
@@ -6187,7 +6355,7 @@
         <v>cvcomnt varchar (255),</v>
       </c>
     </row>
-    <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>287</v>
       </c>
@@ -6223,7 +6391,7 @@
         <v>cdcrjfields varchar (100),</v>
       </c>
     </row>
-    <row r="89" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>287</v>
       </c>
@@ -6264,7 +6432,7 @@
         <v>cdclst smallint check (cdclst &gt;=0 and cdclst &lt;=1),</v>
       </c>
     </row>
-    <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>303</v>
       </c>
@@ -6306,7 +6474,7 @@
         <v>aum integer,</v>
       </c>
     </row>
-    <row r="91" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>303</v>
       </c>
@@ -6348,7 +6516,7 @@
         <v xml:space="preserve">atitle smallint, </v>
       </c>
     </row>
-    <row r="92" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>303</v>
       </c>
@@ -6381,7 +6549,7 @@
         <v>aa1 varchar (800),</v>
       </c>
     </row>
-    <row r="93" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>303</v>
       </c>
@@ -6414,7 +6582,7 @@
         <v>aa2 varchar (800),</v>
       </c>
     </row>
-    <row r="94" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>303</v>
       </c>
@@ -6447,7 +6615,7 @@
         <v>aa3 varchar (800),</v>
       </c>
     </row>
-    <row r="95" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>303</v>
       </c>
@@ -6480,7 +6648,7 @@
         <v>aa4 varchar (800),</v>
       </c>
     </row>
-    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>303</v>
       </c>
@@ -6513,7 +6681,7 @@
         <v>aa5 varchar (800),</v>
       </c>
     </row>
-    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>303</v>
       </c>
@@ -6546,7 +6714,7 @@
         <v>aa6 varchar (800),</v>
       </c>
     </row>
-    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>303</v>
       </c>
@@ -6579,7 +6747,7 @@
         <v>aa7 varchar (800),</v>
       </c>
     </row>
-    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>303</v>
       </c>
@@ -6612,7 +6780,7 @@
         <v>aa8 varchar (800),</v>
       </c>
     </row>
-    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>303</v>
       </c>
@@ -6645,7 +6813,7 @@
         <v>aa9 varchar (800),</v>
       </c>
     </row>
-    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>303</v>
       </c>
@@ -6678,7 +6846,7 @@
         <v>aa10 varchar (800),</v>
       </c>
     </row>
-    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>303</v>
       </c>
@@ -6711,7 +6879,7 @@
         <v>aa11 varchar (800),</v>
       </c>
     </row>
-    <row r="103" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>303</v>
       </c>
@@ -6744,7 +6912,7 @@
         <v>aa12 varchar (800),</v>
       </c>
     </row>
-    <row r="104" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>303</v>
       </c>
@@ -6773,8 +6941,8 @@
       <c r="N104" t="s">
         <v>19</v>
       </c>
-      <c r="P104" t="s">
-        <v>302</v>
+      <c r="P104" s="14" t="s">
+        <v>500</v>
       </c>
       <c r="Q104" t="s">
         <v>306</v>
@@ -6788,7 +6956,7 @@
         <v>optpst smallint check (optpst &gt;=0 and optpst &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="105" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>303</v>
       </c>
@@ -6817,8 +6985,8 @@
       <c r="N105" t="s">
         <v>19</v>
       </c>
-      <c r="P105" t="s">
-        <v>302</v>
+      <c r="P105" s="14" t="s">
+        <v>500</v>
       </c>
       <c r="Q105" t="s">
         <v>306</v>
@@ -6832,7 +7000,7 @@
         <v>optph smallint check (optph &gt;=0 and optph &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>303</v>
       </c>
@@ -6861,8 +7029,8 @@
       <c r="N106" t="s">
         <v>19</v>
       </c>
-      <c r="P106" t="s">
-        <v>302</v>
+      <c r="P106" s="14" t="s">
+        <v>500</v>
       </c>
       <c r="Q106" t="s">
         <v>361</v>
@@ -6876,7 +7044,7 @@
         <v>optin smallint check (optin &gt;=0 and optin &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>303</v>
       </c>
@@ -6905,8 +7073,8 @@
       <c r="N107" t="s">
         <v>19</v>
       </c>
-      <c r="P107" t="s">
-        <v>302</v>
+      <c r="P107" s="14" t="s">
+        <v>500</v>
       </c>
       <c r="Q107" t="s">
         <v>306</v>
@@ -6920,7 +7088,7 @@
         <v>opteml smallint check (opteml &gt;=0 and opteml &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>303</v>
       </c>
@@ -6946,8 +7114,8 @@
       <c r="N108" t="s">
         <v>19</v>
       </c>
-      <c r="P108" t="s">
-        <v>302</v>
+      <c r="P108" s="14" t="s">
+        <v>500</v>
       </c>
       <c r="R108" t="str">
         <f t="shared" ref="R108:R109" si="8">"smallint check ("&amp;I108&amp;" &gt;=0 and "&amp;I108&amp;" &lt;=1),"</f>
@@ -6958,7 +7126,7 @@
         <v>dnd smallint check (dnd &gt;=0 and dnd &lt;=1),</v>
       </c>
     </row>
-    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>366</v>
       </c>
@@ -6984,8 +7152,8 @@
       <c r="N109" t="s">
         <v>19</v>
       </c>
-      <c r="P109" t="s">
-        <v>369</v>
+      <c r="P109" s="14" t="s">
+        <v>500</v>
       </c>
       <c r="R109" t="str">
         <f t="shared" si="8"/>
@@ -6996,22 +7164,21 @@
         <v>cvdisp smallint check (cvdisp &gt;=0 and cvdisp &lt;=1),</v>
       </c>
     </row>
-    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="111" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>287</v>
       </c>
       <c r="C111" t="s">
+        <v>369</v>
+      </c>
+      <c r="D111" t="s">
         <v>370</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E111" t="s">
+        <v>19</v>
+      </c>
+      <c r="I111" t="s">
         <v>371</v>
-      </c>
-      <c r="E111" t="s">
-        <v>19</v>
-      </c>
-      <c r="I111" t="s">
-        <v>372</v>
       </c>
       <c r="J111" t="s">
         <v>51</v>
@@ -7033,21 +7200,21 @@
         <v>cdcsvagti integer,</v>
       </c>
     </row>
-    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>287</v>
       </c>
       <c r="C112" t="s">
+        <v>372</v>
+      </c>
+      <c r="D112" t="s">
+        <v>370</v>
+      </c>
+      <c r="E112" t="s">
+        <v>19</v>
+      </c>
+      <c r="I112" t="s">
         <v>373</v>
-      </c>
-      <c r="D112" t="s">
-        <v>371</v>
-      </c>
-      <c r="E112" t="s">
-        <v>19</v>
-      </c>
-      <c r="I112" t="s">
-        <v>374</v>
       </c>
       <c r="L112" t="s">
         <v>188</v>
@@ -7060,15 +7227,15 @@
         <v>cdcsvdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="113" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>287</v>
       </c>
       <c r="C113" t="s">
+        <v>374</v>
+      </c>
+      <c r="D113" t="s">
         <v>375</v>
-      </c>
-      <c r="D113" t="s">
-        <v>376</v>
       </c>
       <c r="E113" t="s">
         <v>20</v>
@@ -7077,7 +7244,7 @@
         <v>203</v>
       </c>
       <c r="I113" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K113" s="3"/>
       <c r="L113" t="s">
@@ -7087,7 +7254,7 @@
         <v>19</v>
       </c>
       <c r="P113" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="R113" t="str">
         <f>"smallint check ("&amp;I113&amp;" &gt;=0 and "&amp;I113&amp;" &lt;=1),"</f>
@@ -7098,21 +7265,21 @@
         <v>cdcsv smallint check (cdcsv &gt;=0 and cdcsv &lt;=1),</v>
       </c>
     </row>
-    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>287</v>
       </c>
       <c r="C114" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D114" t="s">
+        <v>378</v>
+      </c>
+      <c r="E114" t="s">
+        <v>19</v>
+      </c>
+      <c r="I114" t="s">
         <v>379</v>
-      </c>
-      <c r="E114" t="s">
-        <v>19</v>
-      </c>
-      <c r="I114" t="s">
-        <v>380</v>
       </c>
       <c r="J114" t="s">
         <v>51</v>
@@ -7127,7 +7294,7 @@
         <v>20</v>
       </c>
       <c r="Q114" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R114" t="s">
         <v>43</v>
@@ -7137,27 +7304,27 @@
         <v>cdcsbagti integer,</v>
       </c>
     </row>
-    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>287</v>
       </c>
       <c r="C115" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D115" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E115" t="s">
         <v>19</v>
       </c>
       <c r="I115" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="L115" t="s">
         <v>188</v>
       </c>
       <c r="Q115" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R115" t="s">
         <v>189</v>
@@ -7167,21 +7334,21 @@
         <v>cdcsbdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>287</v>
       </c>
       <c r="C116" t="s">
+        <v>382</v>
+      </c>
+      <c r="D116" t="s">
+        <v>378</v>
+      </c>
+      <c r="E116" t="s">
+        <v>19</v>
+      </c>
+      <c r="I116" t="s">
         <v>383</v>
-      </c>
-      <c r="D116" t="s">
-        <v>379</v>
-      </c>
-      <c r="E116" t="s">
-        <v>19</v>
-      </c>
-      <c r="I116" t="s">
-        <v>384</v>
       </c>
       <c r="J116" t="s">
         <v>51</v>
@@ -7196,7 +7363,7 @@
         <v>20</v>
       </c>
       <c r="Q116" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R116" t="s">
         <v>43</v>
@@ -7206,27 +7373,27 @@
         <v>cdcsbagtii integer,</v>
       </c>
     </row>
-    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>287</v>
       </c>
       <c r="C117" t="s">
+        <v>385</v>
+      </c>
+      <c r="D117" t="s">
+        <v>378</v>
+      </c>
+      <c r="E117" t="s">
+        <v>19</v>
+      </c>
+      <c r="I117" t="s">
         <v>386</v>
-      </c>
-      <c r="D117" t="s">
-        <v>379</v>
-      </c>
-      <c r="E117" t="s">
-        <v>19</v>
-      </c>
-      <c r="I117" t="s">
-        <v>387</v>
       </c>
       <c r="L117" t="s">
         <v>188</v>
       </c>
       <c r="Q117" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R117" t="s">
         <v>189</v>
@@ -7236,21 +7403,21 @@
         <v>cdcsbdtii timestamp without time zone,</v>
       </c>
     </row>
-    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>287</v>
       </c>
       <c r="C118" t="s">
+        <v>387</v>
+      </c>
+      <c r="D118" t="s">
         <v>388</v>
       </c>
-      <c r="D118" t="s">
+      <c r="E118" t="s">
+        <v>19</v>
+      </c>
+      <c r="I118" t="s">
         <v>389</v>
-      </c>
-      <c r="E118" t="s">
-        <v>19</v>
-      </c>
-      <c r="I118" t="s">
-        <v>390</v>
       </c>
       <c r="J118" t="s">
         <v>51</v>
@@ -7265,7 +7432,7 @@
         <v>20</v>
       </c>
       <c r="Q118" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="R118" t="s">
         <v>43</v>
@@ -7275,27 +7442,27 @@
         <v>cdcrjtagti integer,</v>
       </c>
     </row>
-    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>287</v>
       </c>
       <c r="C119" t="s">
+        <v>391</v>
+      </c>
+      <c r="D119" t="s">
+        <v>388</v>
+      </c>
+      <c r="E119" t="s">
+        <v>19</v>
+      </c>
+      <c r="I119" t="s">
         <v>392</v>
-      </c>
-      <c r="D119" t="s">
-        <v>389</v>
-      </c>
-      <c r="E119" t="s">
-        <v>19</v>
-      </c>
-      <c r="I119" t="s">
-        <v>393</v>
       </c>
       <c r="L119" t="s">
         <v>188</v>
       </c>
       <c r="Q119" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="R119" t="s">
         <v>189</v>
@@ -7305,21 +7472,21 @@
         <v>cdcrjtdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>287</v>
       </c>
       <c r="C120" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D120" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E120" t="s">
         <v>19</v>
       </c>
       <c r="I120" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J120" t="s">
         <v>51</v>
@@ -7334,7 +7501,7 @@
         <v>20</v>
       </c>
       <c r="Q120" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="R120" t="s">
         <v>43</v>
@@ -7344,27 +7511,27 @@
         <v>cdcrjtagtii integer,</v>
       </c>
     </row>
-    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>287</v>
       </c>
       <c r="C121" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D121" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E121" t="s">
         <v>19</v>
       </c>
       <c r="I121" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L121" t="s">
         <v>188</v>
       </c>
       <c r="Q121" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="R121" t="s">
         <v>189</v>
@@ -7374,15 +7541,15 @@
         <v>cdcrjtdtii timestamp without time zone,</v>
       </c>
     </row>
-    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>287</v>
       </c>
       <c r="C122" t="s">
+        <v>396</v>
+      </c>
+      <c r="D122" t="s">
         <v>397</v>
-      </c>
-      <c r="D122" t="s">
-        <v>398</v>
       </c>
       <c r="E122" t="s">
         <v>20</v>
@@ -7391,7 +7558,7 @@
         <v>203</v>
       </c>
       <c r="I122" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K122" s="3"/>
       <c r="L122" s="9" t="s">
@@ -7401,7 +7568,7 @@
         <v>19</v>
       </c>
       <c r="P122" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="R122" t="str">
         <f t="shared" ref="R122:R123" si="10">"smallint check ("&amp;I122&amp;" &gt;=0 and "&amp;I122&amp;" &lt;=4),"</f>
@@ -7412,15 +7579,15 @@
         <v>cdcsb smallint check (cdcsb &gt;=0 and cdcsb &lt;=4),</v>
       </c>
     </row>
-    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>287</v>
       </c>
       <c r="C123" t="s">
+        <v>400</v>
+      </c>
+      <c r="D123" t="s">
         <v>401</v>
-      </c>
-      <c r="D123" t="s">
-        <v>402</v>
       </c>
       <c r="E123" t="s">
         <v>20</v>
@@ -7429,7 +7596,7 @@
         <v>203</v>
       </c>
       <c r="I123" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K123" s="3"/>
       <c r="L123" t="s">
@@ -7439,7 +7606,7 @@
         <v>19</v>
       </c>
       <c r="P123" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="R123" t="str">
         <f t="shared" si="10"/>
@@ -7450,21 +7617,21 @@
         <v>cdcrjt smallint check (cdcrjt &gt;=0 and cdcrjt &lt;=4),</v>
       </c>
     </row>
-    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>287</v>
       </c>
       <c r="C124" t="s">
+        <v>404</v>
+      </c>
+      <c r="D124" t="s">
         <v>405</v>
       </c>
-      <c r="D124" t="s">
+      <c r="E124" t="s">
+        <v>19</v>
+      </c>
+      <c r="I124" t="s">
         <v>406</v>
-      </c>
-      <c r="E124" t="s">
-        <v>19</v>
-      </c>
-      <c r="I124" t="s">
-        <v>407</v>
       </c>
       <c r="K124" s="3"/>
       <c r="L124" t="s">
@@ -7477,7 +7644,7 @@
         <v>81</v>
       </c>
       <c r="P124" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="R124" t="str">
         <f>"smallint check ("&amp;I124&amp;" &gt;=0 and "&amp;I124&amp;" &lt;=2),"</f>
@@ -7488,21 +7655,21 @@
         <v>cdccomp smallint check (cdccomp &gt;=0 and cdccomp &lt;=2),</v>
       </c>
     </row>
-    <row r="125" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>287</v>
       </c>
       <c r="C125" t="s">
+        <v>408</v>
+      </c>
+      <c r="D125" t="s">
         <v>409</v>
       </c>
-      <c r="D125" t="s">
+      <c r="E125" t="s">
+        <v>19</v>
+      </c>
+      <c r="I125" t="s">
         <v>410</v>
-      </c>
-      <c r="E125" t="s">
-        <v>19</v>
-      </c>
-      <c r="I125" t="s">
-        <v>411</v>
       </c>
       <c r="K125" s="3"/>
       <c r="L125" t="s">
@@ -7529,12 +7696,12 @@
         <v>cdcmandt smallint check (cdcmandt &gt;=0 and cdcmandt &lt;=1),</v>
       </c>
     </row>
-    <row r="126" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>287</v>
       </c>
       <c r="C126" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E126" t="s">
         <v>19</v>
@@ -7543,7 +7710,7 @@
         <v>203</v>
       </c>
       <c r="I126" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K126" s="3"/>
       <c r="L126" t="s">
@@ -7564,23 +7731,23 @@
         <v>cdcload smallint check (cdcload &gt;=0 and cdcload &lt;=1),</v>
       </c>
     </row>
-    <row r="127" spans="1:20" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:20" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>366</v>
       </c>
       <c r="C129" t="s">
+        <v>413</v>
+      </c>
+      <c r="D129" t="s">
         <v>414</v>
       </c>
-      <c r="D129" t="s">
+      <c r="E129" t="s">
+        <v>19</v>
+      </c>
+      <c r="I129" t="s">
         <v>415</v>
-      </c>
-      <c r="E129" t="s">
-        <v>19</v>
-      </c>
-      <c r="I129" t="s">
-        <v>416</v>
       </c>
       <c r="L129" t="s">
         <v>22</v>
@@ -7596,21 +7763,21 @@
         <v>lsagti integer,</v>
       </c>
     </row>
-    <row r="130" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>366</v>
       </c>
       <c r="C130" t="s">
+        <v>416</v>
+      </c>
+      <c r="D130" t="s">
         <v>417</v>
       </c>
-      <c r="D130" t="s">
+      <c r="E130" t="s">
+        <v>19</v>
+      </c>
+      <c r="I130" t="s">
         <v>418</v>
-      </c>
-      <c r="E130" t="s">
-        <v>19</v>
-      </c>
-      <c r="I130" t="s">
-        <v>419</v>
       </c>
       <c r="L130" t="s">
         <v>188</v>
@@ -7623,15 +7790,15 @@
         <v>lsdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>366</v>
       </c>
       <c r="C131" t="s">
+        <v>419</v>
+      </c>
+      <c r="D131" t="s">
         <v>420</v>
-      </c>
-      <c r="D131" t="s">
-        <v>421</v>
       </c>
       <c r="E131" t="s">
         <v>20</v>
@@ -7640,7 +7807,7 @@
         <v>62</v>
       </c>
       <c r="I131" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L131" t="s">
         <v>47</v>
@@ -7656,15 +7823,15 @@
         <v>lscomnti varchar (255),</v>
       </c>
     </row>
-    <row r="132" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>422</v>
+      </c>
+      <c r="C132" t="s">
         <v>423</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>424</v>
-      </c>
-      <c r="D132" t="s">
-        <v>425</v>
       </c>
       <c r="E132" t="s">
         <v>20</v>
@@ -7676,7 +7843,7 @@
         <v>20</v>
       </c>
       <c r="I132" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K132" s="3"/>
       <c r="L132" t="s">
@@ -7700,15 +7867,15 @@
         <v>clscored smallint check (clscored &gt;=0 and clscored &lt;=1) not null,</v>
       </c>
     </row>
-    <row r="133" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>366</v>
       </c>
       <c r="C133" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D133" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E133" t="s">
         <v>20</v>
@@ -7720,7 +7887,7 @@
         <v>20</v>
       </c>
       <c r="I133" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K133" s="3"/>
       <c r="L133" t="s">
@@ -7730,10 +7897,10 @@
         <v>19</v>
       </c>
       <c r="P133" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q133" t="s">
         <v>429</v>
-      </c>
-      <c r="Q133" t="s">
-        <v>430</v>
       </c>
       <c r="R133" t="str">
         <f t="shared" ref="R133:R134" si="13">"smallint check ("&amp;I133&amp;" &gt;=0 and "&amp;I133&amp;" &lt;=1),"</f>
@@ -7744,12 +7911,12 @@
         <v>cdctg smallint check (cdctg &gt;=0 and cdctg &lt;=1),</v>
       </c>
     </row>
-    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>366</v>
       </c>
       <c r="C134" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E134" t="s">
         <v>19</v>
@@ -7758,7 +7925,7 @@
         <v>203</v>
       </c>
       <c r="I134" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K134" s="3"/>
       <c r="L134" t="s">
@@ -7779,26 +7946,26 @@
         <v>lsload smallint check (lsload &gt;=0 and lsload &lt;=1),</v>
       </c>
     </row>
-    <row r="135" spans="1:20" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="136" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:20" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="136" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>432</v>
+      </c>
+      <c r="C137" t="s">
         <v>433</v>
       </c>
-      <c r="C137" t="s">
+      <c r="D137" t="s">
         <v>434</v>
       </c>
-      <c r="D137" t="s">
+      <c r="E137" t="s">
+        <v>19</v>
+      </c>
+      <c r="G137" t="s">
+        <v>20</v>
+      </c>
+      <c r="I137" t="s">
         <v>435</v>
-      </c>
-      <c r="E137" t="s">
-        <v>19</v>
-      </c>
-      <c r="G137" t="s">
-        <v>20</v>
-      </c>
-      <c r="I137" t="s">
-        <v>436</v>
       </c>
       <c r="K137" s="3"/>
       <c r="L137" t="s">
@@ -7808,7 +7975,7 @@
         <v>19</v>
       </c>
       <c r="P137" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="R137" t="str">
         <f t="shared" ref="R137:R142" si="14">"smallint check ("&amp;I137&amp;" &gt;=0 and "&amp;I137&amp;" &lt;=1),"</f>
@@ -7819,15 +7986,15 @@
         <v>qaload smallint check (qaload &gt;=0 and qaload &lt;=1),</v>
       </c>
     </row>
-    <row r="138" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C138" t="s">
+        <v>437</v>
+      </c>
+      <c r="D138" t="s">
         <v>438</v>
-      </c>
-      <c r="D138" t="s">
-        <v>439</v>
       </c>
       <c r="E138" t="s">
         <v>20</v>
@@ -7839,7 +8006,7 @@
         <v>20</v>
       </c>
       <c r="I138" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K138" s="3"/>
       <c r="L138" t="s">
@@ -7849,7 +8016,7 @@
         <v>19</v>
       </c>
       <c r="P138" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="R138" t="str">
         <f t="shared" si="14"/>
@@ -7860,15 +8027,15 @@
         <v>qadcrej smallint check (qadcrej &gt;=0 and qadcrej &lt;=1),</v>
       </c>
     </row>
-    <row r="139" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C139" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D139" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E139" t="s">
         <v>20</v>
@@ -7880,7 +8047,7 @@
         <v>20</v>
       </c>
       <c r="I139" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K139" s="3"/>
       <c r="L139" t="s">
@@ -7890,10 +8057,10 @@
         <v>19</v>
       </c>
       <c r="P139" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Q139" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R139" t="str">
         <f t="shared" si="14"/>
@@ -7904,15 +8071,15 @@
         <v>qacdcrej smallint check (qacdcrej &gt;=0 and qacdcrej &lt;=1),</v>
       </c>
     </row>
-    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C140" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D140" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E140" t="s">
         <v>20</v>
@@ -7924,7 +8091,7 @@
         <v>20</v>
       </c>
       <c r="I140" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K140" s="3"/>
       <c r="L140" t="s">
@@ -7934,7 +8101,7 @@
         <v>19</v>
       </c>
       <c r="P140" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="R140" t="str">
         <f t="shared" si="14"/>
@@ -7945,15 +8112,15 @@
         <v>qarej smallint check (qarej &gt;=0 and qarej &lt;=1),</v>
       </c>
     </row>
-    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C141" t="s">
+        <v>446</v>
+      </c>
+      <c r="D141" t="s">
         <v>447</v>
-      </c>
-      <c r="D141" t="s">
-        <v>448</v>
       </c>
       <c r="E141" t="s">
         <v>20</v>
@@ -7965,7 +8132,7 @@
         <v>20</v>
       </c>
       <c r="I141" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K141" s="3"/>
       <c r="L141" t="s">
@@ -7975,7 +8142,7 @@
         <v>19</v>
       </c>
       <c r="P141" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="R141" t="str">
         <f t="shared" si="14"/>
@@ -7986,15 +8153,15 @@
         <v>qaacpt smallint check (qaacpt &gt;=0 and qaacpt &lt;=1),</v>
       </c>
     </row>
-    <row r="142" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C142" t="s">
+        <v>450</v>
+      </c>
+      <c r="D142" t="s">
         <v>451</v>
-      </c>
-      <c r="D142" t="s">
-        <v>452</v>
       </c>
       <c r="E142" t="s">
         <v>20</v>
@@ -8006,7 +8173,7 @@
         <v>20</v>
       </c>
       <c r="I142" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K142" s="3"/>
       <c r="L142" t="s">
@@ -8016,7 +8183,7 @@
         <v>19</v>
       </c>
       <c r="P142" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="R142" t="str">
         <f t="shared" si="14"/>
@@ -8027,15 +8194,15 @@
         <v>qasv smallint check (qasv &gt;=0 and qasv &lt;=1),</v>
       </c>
     </row>
-    <row r="143" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C143" t="s">
+        <v>453</v>
+      </c>
+      <c r="D143" t="s">
         <v>454</v>
-      </c>
-      <c r="D143" t="s">
-        <v>455</v>
       </c>
       <c r="E143" t="s">
         <v>20</v>
@@ -8047,7 +8214,7 @@
         <v>20</v>
       </c>
       <c r="I143" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L143" t="s">
         <v>47</v>
@@ -8056,7 +8223,7 @@
         <v>25</v>
       </c>
       <c r="P143" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="R143" t="s">
         <v>292</v>
@@ -8066,22 +8233,21 @@
         <v>qastat varchar (25),</v>
       </c>
     </row>
-    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="145" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C145" t="s">
+        <v>457</v>
+      </c>
+      <c r="D145" t="s">
         <v>458</v>
       </c>
-      <c r="D145" t="s">
+      <c r="E145" t="s">
+        <v>19</v>
+      </c>
+      <c r="I145" t="s">
         <v>459</v>
-      </c>
-      <c r="E145" t="s">
-        <v>19</v>
-      </c>
-      <c r="I145" t="s">
-        <v>460</v>
       </c>
       <c r="J145" t="s">
         <v>51</v>
@@ -8096,7 +8262,7 @@
         <v>20</v>
       </c>
       <c r="Q145" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="R145" t="s">
         <v>43</v>
@@ -8106,27 +8272,27 @@
         <v>qarjtagti integer,</v>
       </c>
     </row>
-    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C146" t="s">
+        <v>461</v>
+      </c>
+      <c r="D146" t="s">
+        <v>458</v>
+      </c>
+      <c r="E146" t="s">
+        <v>19</v>
+      </c>
+      <c r="I146" t="s">
         <v>462</v>
-      </c>
-      <c r="D146" t="s">
-        <v>459</v>
-      </c>
-      <c r="E146" t="s">
-        <v>19</v>
-      </c>
-      <c r="I146" t="s">
-        <v>463</v>
       </c>
       <c r="L146" t="s">
         <v>188</v>
       </c>
       <c r="Q146" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="R146" t="s">
         <v>189</v>
@@ -8136,21 +8302,21 @@
         <v>qarjtdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="147" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C147" t="s">
+        <v>463</v>
+      </c>
+      <c r="D147" t="s">
+        <v>458</v>
+      </c>
+      <c r="E147" t="s">
+        <v>19</v>
+      </c>
+      <c r="I147" t="s">
         <v>464</v>
-      </c>
-      <c r="D147" t="s">
-        <v>459</v>
-      </c>
-      <c r="E147" t="s">
-        <v>19</v>
-      </c>
-      <c r="I147" t="s">
-        <v>465</v>
       </c>
       <c r="J147" t="s">
         <v>51</v>
@@ -8165,7 +8331,7 @@
         <v>20</v>
       </c>
       <c r="Q147" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="R147" t="s">
         <v>43</v>
@@ -8175,27 +8341,27 @@
         <v>qarjtagtii integer,</v>
       </c>
     </row>
-    <row r="148" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C148" t="s">
+        <v>466</v>
+      </c>
+      <c r="D148" t="s">
+        <v>458</v>
+      </c>
+      <c r="E148" t="s">
+        <v>19</v>
+      </c>
+      <c r="I148" t="s">
         <v>467</v>
-      </c>
-      <c r="D148" t="s">
-        <v>459</v>
-      </c>
-      <c r="E148" t="s">
-        <v>19</v>
-      </c>
-      <c r="I148" t="s">
-        <v>468</v>
       </c>
       <c r="L148" t="s">
         <v>188</v>
       </c>
       <c r="Q148" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="R148" t="s">
         <v>189</v>
@@ -8205,21 +8371,21 @@
         <v>qarjtdtii timestamp without time zone,</v>
       </c>
     </row>
-    <row r="149" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C149" t="s">
+        <v>468</v>
+      </c>
+      <c r="D149" t="s">
         <v>469</v>
       </c>
-      <c r="D149" t="s">
+      <c r="E149" t="s">
+        <v>19</v>
+      </c>
+      <c r="I149" t="s">
         <v>470</v>
-      </c>
-      <c r="E149" t="s">
-        <v>19</v>
-      </c>
-      <c r="I149" t="s">
-        <v>471</v>
       </c>
       <c r="J149" t="s">
         <v>51</v>
@@ -8234,7 +8400,7 @@
         <v>20</v>
       </c>
       <c r="Q149" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="R149" t="s">
         <v>43</v>
@@ -8244,27 +8410,27 @@
         <v>qaacptagti integer,</v>
       </c>
     </row>
-    <row r="150" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C150" t="s">
+        <v>472</v>
+      </c>
+      <c r="D150" t="s">
+        <v>469</v>
+      </c>
+      <c r="E150" t="s">
+        <v>19</v>
+      </c>
+      <c r="I150" t="s">
         <v>473</v>
-      </c>
-      <c r="D150" t="s">
-        <v>470</v>
-      </c>
-      <c r="E150" t="s">
-        <v>19</v>
-      </c>
-      <c r="I150" t="s">
-        <v>474</v>
       </c>
       <c r="L150" t="s">
         <v>188</v>
       </c>
       <c r="Q150" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="R150" t="s">
         <v>189</v>
@@ -8274,21 +8440,21 @@
         <v>qaacptdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="151" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C151" t="s">
+        <v>474</v>
+      </c>
+      <c r="D151" t="s">
+        <v>469</v>
+      </c>
+      <c r="E151" t="s">
+        <v>19</v>
+      </c>
+      <c r="I151" t="s">
         <v>475</v>
-      </c>
-      <c r="D151" t="s">
-        <v>470</v>
-      </c>
-      <c r="E151" t="s">
-        <v>19</v>
-      </c>
-      <c r="I151" t="s">
-        <v>476</v>
       </c>
       <c r="J151" t="s">
         <v>51</v>
@@ -8303,7 +8469,7 @@
         <v>20</v>
       </c>
       <c r="Q151" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="R151" t="s">
         <v>43</v>
@@ -8313,27 +8479,27 @@
         <v>qaacptagtii integer,</v>
       </c>
     </row>
-    <row r="152" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C152" t="s">
+        <v>477</v>
+      </c>
+      <c r="D152" t="s">
+        <v>469</v>
+      </c>
+      <c r="E152" t="s">
+        <v>19</v>
+      </c>
+      <c r="I152" t="s">
         <v>478</v>
-      </c>
-      <c r="D152" t="s">
-        <v>470</v>
-      </c>
-      <c r="E152" t="s">
-        <v>19</v>
-      </c>
-      <c r="I152" t="s">
-        <v>479</v>
       </c>
       <c r="L152" t="s">
         <v>188</v>
       </c>
       <c r="Q152" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="R152" t="s">
         <v>189</v>
@@ -8343,21 +8509,21 @@
         <v>qaacptdtii timestamp without time zone,</v>
       </c>
     </row>
-    <row r="153" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C153" t="s">
+        <v>479</v>
+      </c>
+      <c r="D153" t="s">
         <v>480</v>
       </c>
-      <c r="D153" t="s">
+      <c r="E153" t="s">
+        <v>19</v>
+      </c>
+      <c r="I153" t="s">
         <v>481</v>
-      </c>
-      <c r="E153" t="s">
-        <v>19</v>
-      </c>
-      <c r="I153" t="s">
-        <v>482</v>
       </c>
       <c r="J153" t="s">
         <v>51</v>
@@ -8372,7 +8538,7 @@
         <v>20</v>
       </c>
       <c r="Q153" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="R153" t="s">
         <v>43</v>
@@ -8382,27 +8548,27 @@
         <v>qasvagti integer,</v>
       </c>
     </row>
-    <row r="154" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C154" t="s">
+        <v>483</v>
+      </c>
+      <c r="D154" t="s">
+        <v>480</v>
+      </c>
+      <c r="E154" t="s">
+        <v>19</v>
+      </c>
+      <c r="I154" t="s">
         <v>484</v>
-      </c>
-      <c r="D154" t="s">
-        <v>481</v>
-      </c>
-      <c r="E154" t="s">
-        <v>19</v>
-      </c>
-      <c r="I154" t="s">
-        <v>485</v>
       </c>
       <c r="L154" t="s">
         <v>188</v>
       </c>
       <c r="Q154" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="R154" t="s">
         <v>189</v>
@@ -8412,17 +8578,17 @@
         <v>qasvdti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="155" spans="1:20" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="156" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="157" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:20" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="156" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>485</v>
+      </c>
+      <c r="C157" t="s">
         <v>486</v>
       </c>
-      <c r="C157" t="s">
-        <v>487</v>
-      </c>
       <c r="D157" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E157" t="s">
         <v>20</v>
@@ -8431,7 +8597,7 @@
         <v>56</v>
       </c>
       <c r="I157" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K157" s="3"/>
       <c r="L157" t="s">
@@ -8455,21 +8621,21 @@
         <v>dstat smallint check (dstat &gt;=0 and dstat &lt;=1),</v>
       </c>
     </row>
-    <row r="158" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C158" t="s">
+        <v>488</v>
+      </c>
+      <c r="D158" t="s">
         <v>489</v>
       </c>
-      <c r="D158" t="s">
+      <c r="E158" t="s">
+        <v>19</v>
+      </c>
+      <c r="I158" t="s">
         <v>490</v>
-      </c>
-      <c r="E158" t="s">
-        <v>19</v>
-      </c>
-      <c r="I158" t="s">
-        <v>491</v>
       </c>
       <c r="L158" t="s">
         <v>188</v>
@@ -8482,21 +8648,21 @@
         <v>dydti timestamp without time zone,</v>
       </c>
     </row>
-    <row r="159" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C159" t="s">
+        <v>491</v>
+      </c>
+      <c r="D159" t="s">
         <v>492</v>
       </c>
-      <c r="D159" t="s">
+      <c r="E159" t="s">
+        <v>19</v>
+      </c>
+      <c r="I159" t="s">
         <v>493</v>
-      </c>
-      <c r="E159" t="s">
-        <v>19</v>
-      </c>
-      <c r="I159" t="s">
-        <v>494</v>
       </c>
       <c r="L159" t="s">
         <v>22</v>
@@ -8512,21 +8678,21 @@
         <v>dyagti integer,</v>
       </c>
     </row>
-    <row r="160" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C160" t="s">
+        <v>494</v>
+      </c>
+      <c r="D160" t="s">
         <v>495</v>
       </c>
-      <c r="D160" t="s">
+      <c r="E160" t="s">
+        <v>19</v>
+      </c>
+      <c r="I160" t="s">
         <v>496</v>
-      </c>
-      <c r="E160" t="s">
-        <v>19</v>
-      </c>
-      <c r="I160" t="s">
-        <v>497</v>
       </c>
       <c r="K160" s="3"/>
       <c r="L160" t="s">
@@ -8547,38 +8713,28 @@
         <v>dytg smallint check (dytg &gt;=0 and dytg &lt;=1),</v>
       </c>
     </row>
-    <row r="161" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>29</v>
       </c>
       <c r="Q161" s="9"/>
       <c r="T161" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="162" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>29</v>
       </c>
       <c r="Q162" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="T162" t="s">
         <v>499</v>
       </c>
-      <c r="T162" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="163" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="164" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="165" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="166" spans="1:20" hidden="1" x14ac:dyDescent="0.35"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:R166" xr:uid="{0533A871-86A0-4AD7-948B-2DF2F184C401}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="prospect"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:R166" xr:uid="{0533A871-86A0-4AD7-948B-2DF2F184C401}"/>
   <conditionalFormatting sqref="I38 I28">
     <cfRule type="duplicateValues" dxfId="96" priority="91"/>
   </conditionalFormatting>
@@ -8872,5 +9028,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>